<commit_message>
putting everything to git
</commit_message>
<xml_diff>
--- a/main/data/TestData.xlsx
+++ b/main/data/TestData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,11 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Memory Usage (bytes)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Error Message</t>
         </is>
       </c>
@@ -468,9 +473,12 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.4630088806152344</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
+        <v>18.96929740905762</v>
+      </c>
+      <c r="E2" t="n">
+        <v>99031</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -485,9 +493,72 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.01120567321777344</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
+        <v>16.99519157409668</v>
+      </c>
+      <c r="E3" t="n">
+        <v>87336</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Success 🟢</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>20.84207534790039</v>
+      </c>
+      <c r="E4" t="n">
+        <v>87248</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Success 🟢</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>16.85214042663574</v>
+      </c>
+      <c r="E5" t="n">
+        <v>87248</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Success 🟢</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>16.95394515991211</v>
+      </c>
+      <c r="E6" t="n">
+        <v>87248</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>